<commit_message>
salary graphs and some other things
</commit_message>
<xml_diff>
--- a/server/uploads/documents/salary.xlsx
+++ b/server/uploads/documents/salary.xlsx
@@ -121,20 +121,24 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="5">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="2" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="false" applyBorder="true" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="false" applyBorder="true" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="2" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="false" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="false" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -390,72 +394,72 @@
   <dimension ref="A1:D4"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B2" activeCellId="0" sqref="B2"/>
+      <selection pane="topLeft" activeCell="D8" activeCellId="0" sqref="D8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.6015625" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="18.43"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="14"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="21.71"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="19.43"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="18.29"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="18.43"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="14"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="1" width="21.71"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="1" width="16.87"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="1" width="18.29"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1" s="1" t="s">
+      <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="B1" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="C1" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="D1" s="2" t="s">
         <v>3</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="2" t="n">
-        <v>12</v>
-      </c>
-      <c r="B2" s="2" t="n">
-        <v>450</v>
-      </c>
-      <c r="C2" s="3" t="n">
-        <v>45047</v>
-      </c>
-      <c r="D2" s="2" t="n">
-        <v>4</v>
+      <c r="A2" s="3" t="n">
+        <v>33</v>
+      </c>
+      <c r="B2" s="3" t="n">
+        <v>1450</v>
+      </c>
+      <c r="C2" s="4" t="n">
+        <v>45052</v>
+      </c>
+      <c r="D2" s="3" t="n">
+        <v>2</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="2" t="n">
-        <v>13</v>
-      </c>
-      <c r="B3" s="2" t="n">
-        <v>500</v>
-      </c>
-      <c r="C3" s="3" t="n">
-        <v>45048</v>
-      </c>
-      <c r="D3" s="2" t="n">
-        <v>4</v>
+      <c r="A3" s="3" t="n">
+        <v>34</v>
+      </c>
+      <c r="B3" s="3" t="n">
+        <v>1000</v>
+      </c>
+      <c r="C3" s="4" t="n">
+        <v>45052</v>
+      </c>
+      <c r="D3" s="3" t="n">
+        <v>2</v>
       </c>
     </row>
-    <row r="4" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A4" s="2" t="n">
-        <v>14</v>
-      </c>
-      <c r="B4" s="2" t="n">
-        <v>3000</v>
-      </c>
-      <c r="C4" s="3" t="n">
-        <v>45049</v>
-      </c>
-      <c r="D4" s="2" t="n">
-        <v>4</v>
+    <row r="4" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A4" s="3" t="n">
+        <v>35</v>
+      </c>
+      <c r="B4" s="3" t="n">
+        <v>4000</v>
+      </c>
+      <c r="C4" s="4" t="n">
+        <v>45052</v>
+      </c>
+      <c r="D4" s="3" t="n">
+        <v>2</v>
       </c>
     </row>
   </sheetData>

</xml_diff>